<commit_message>
cleaned up collision file
</commit_message>
<xml_diff>
--- a/collisionMatrix.xlsx
+++ b/collisionMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brendan\Desktop\Projects\game_9_30_20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5B8457-E468-47D9-B7F8-158CF8CF66DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2061622-4103-4846-B1A1-084A622C4F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D700DE0-051A-4FE5-894A-4AB7835514A6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
   <si>
     <t>terrain</t>
   </si>
@@ -490,7 +490,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +659,9 @@
         <v>14</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="G5" s="3"/>
       <c r="H5" s="8" t="s">
         <v>14</v>
@@ -679,7 +681,9 @@
         <v>14</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="8" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
implemented collision for magic and explosions
</commit_message>
<xml_diff>
--- a/collisionMatrix.xlsx
+++ b/collisionMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brendan\Desktop\Projects\game_9_30_20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2061622-4103-4846-B1A1-084A622C4F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D123940-AD23-491A-A599-F707E5230B44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D700DE0-051A-4FE5-894A-4AB7835514A6}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,11 +562,11 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
+      <c r="G2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>14</v>
@@ -699,8 +699,8 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
+      <c r="B7" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="8" t="s">
@@ -724,8 +724,8 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
+      <c r="B8" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>14</v>
@@ -741,8 +741,8 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="5" t="s">
-        <v>11</v>
+      <c r="M8" s="12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -842,8 +842,8 @@
       <c r="G13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>11</v>
+      <c r="H13" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>14</v>

</xml_diff>